<commit_message>
Updates to SYVbT fixing data export issue.
</commit_message>
<xml_diff>
--- a/InputData/trans/SYVbT/Start Year Vehicles by Technology.xlsx
+++ b/InputData/trans/SYVbT/Start Year Vehicles by Technology.xlsx
@@ -2387,9 +2387,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5">
-        <f>B14/SUM(B14:B15)</f>
-        <v/>
+      <c r="A5" t="n">
+        <v>0.7521692785979465</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -2398,9 +2397,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6">
-        <f>1-A5</f>
-        <v/>
+      <c r="A6" t="n">
+        <v>0.2478307214020535</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -2409,9 +2407,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8">
-        <f>SUM(INDEX('AEO 37'!$110:$110,MATCH(About!$B$83,'AEO 37'!$1:$1,0)))/INDEX('AEO 37'!$109:$109,MATCH(About!$B$83,'AEO 37'!$1:$1,0))</f>
-        <v/>
+      <c r="A8" t="n">
+        <v>0.7859711365966666</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -2420,9 +2417,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9">
-        <f>SUM(INDEX('AEO 37'!$111:$111,MATCH(About!$B$83,'AEO 37'!$1:$1,0)))/INDEX('AEO 37'!$109:$109,MATCH(About!$B$83,'AEO 37'!$1:$1,0))</f>
-        <v/>
+      <c r="A9" t="n">
+        <v>0.2140288469287458</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -2799,22 +2795,22 @@
         </is>
       </c>
       <c r="B2" s="20" t="n">
-        <v>5</v>
+        <v>32978</v>
       </c>
       <c r="C2" s="20" t="n">
-        <v>1131</v>
+        <v>1194</v>
       </c>
       <c r="D2" s="20" t="n">
-        <v>50075</v>
+        <v>2739367</v>
       </c>
       <c r="E2" s="20" t="n">
-        <v>127237</v>
+        <v>76202</v>
       </c>
       <c r="F2" s="20" t="n">
-        <v>0</v>
+        <v>29824</v>
       </c>
       <c r="G2" s="20" t="n">
-        <v>2247</v>
+        <v>596</v>
       </c>
       <c r="H2" s="20" t="n">
         <v>0</v>
@@ -2827,32 +2823,26 @@
           <t>HDVs</t>
         </is>
       </c>
-      <c r="B3" s="20">
-        <f>Misc!A3</f>
-        <v/>
-      </c>
-      <c r="C3" s="20">
-        <f>SUM(INDEX('AEO 37'!$75:$75,MATCH(About!$B$83,'AEO 37'!$1:$1,0)),INDEX('AEO 37'!$83:$83,MATCH(About!$B$83,'AEO 37'!$1:$1,0)),INDEX('AEO 37'!$91:$91,MATCH(About!$B$83,'AEO 37'!$1:$1,0)))/INDEX('AEO 37'!$70:$70,MATCH(About!$B$83,'AEO 37'!$1:$1,0))*INDEX('NTS 1-11'!$14:$14,MATCH(About!$B$83,'NTS 1-11'!$2:$2,0))-'SYVbT-freight'!C2</f>
-        <v/>
-      </c>
-      <c r="D3" s="20">
-        <f>SUM(INDEX('AEO 37'!$72:$72,MATCH(About!$B$83,'AEO 37'!$1:$1,0)),INDEX('AEO 37'!$80:$80,MATCH(About!$B$83,'AEO 37'!$1:$1,0)),INDEX('AEO 37'!$88:$88,MATCH(About!$B$83,'AEO 37'!$1:$1,0)))/INDEX('AEO 37'!$70:$70,MATCH(About!$B$83,'AEO 37'!$1:$1,0))*INDEX('NTS 1-11'!$14:$14,MATCH(About!$B$83,'NTS 1-11'!$2:$2,0))</f>
-        <v/>
-      </c>
-      <c r="E3" s="20">
-        <f>SUM(INDEX('AEO 37'!$74:$74,MATCH(About!$B$83,'AEO 37'!$1:$1,0)),INDEX('AEO 37'!$82:$82,MATCH(About!$B$83,'AEO 37'!$1:$1,0)),INDEX('AEO 37'!$90:$90,MATCH(About!$B$83,'AEO 37'!$1:$1,0)))/INDEX('AEO 37'!$70:$70,MATCH(About!$B$83,'AEO 37'!$1:$1,0))*INDEX('NTS 1-11'!$14:$14,MATCH(About!$B$83,'NTS 1-11'!$2:$2,0))</f>
-        <v/>
+      <c r="B3" s="20" t="n">
+        <v>339</v>
+      </c>
+      <c r="C3" s="20" t="n">
+        <v>448</v>
+      </c>
+      <c r="D3" s="20" t="n">
+        <v>20</v>
+      </c>
+      <c r="E3" s="20" t="n">
+        <v>1123</v>
       </c>
       <c r="F3" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="G3" s="20">
-        <f>SUM(INDEX('AEO 37'!$76:$76,MATCH(About!$B$83,'AEO 37'!$1:$1,0)),INDEX('AEO 37'!$84:$84,MATCH(About!$B$83,'AEO 37'!$1:$1,0)),INDEX('AEO 37'!$92:$92,MATCH(About!$B$83,'AEO 37'!$1:$1,0)))/INDEX('AEO 37'!$70:$70,MATCH(About!$B$83,'AEO 37'!$1:$1,0))*INDEX('NTS 1-11'!$14:$14,MATCH(About!$B$83,'NTS 1-11'!$2:$2,0))</f>
-        <v/>
-      </c>
-      <c r="H3" s="20">
-        <f>SUM(INDEX('AEO 37'!$78:$78,MATCH(About!$B$83,'AEO 37'!$1:$1,0)),INDEX('AEO 37'!$86:$86,MATCH(About!$B$83,'AEO 37'!$1:$1,0)),INDEX('AEO 37'!$94:$94,MATCH(About!$B$83,'AEO 37'!$1:$1,0)))/INDEX('AEO 37'!$70:$70,MATCH(About!$B$83,'AEO 37'!$1:$1,0))*INDEX('NTS 1-11'!$14:$14,MATCH(About!$B$83,'NTS 1-11'!$2:$2,0))</f>
-        <v/>
+      <c r="G3" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="20" t="n">
+        <v>0</v>
       </c>
       <c r="I3" s="20" t="n"/>
       <c r="J3" s="115" t="n"/>
@@ -2969,7 +2959,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8"/>
     <row r="9">
       <c r="B9" s="20" t="n"/>
       <c r="C9" s="20" t="n"/>
@@ -2991,7 +2980,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
@@ -3057,33 +3046,26 @@
           <t>LDVs</t>
         </is>
       </c>
-      <c r="B2" s="20">
-        <f>SUM(INDEX('AEO 46'!73:73,0,MATCH(About!$B$83,'AEO 46'!1:1,0)))*10^6</f>
-        <v/>
-      </c>
-      <c r="C2" s="20">
-        <f>SUM(INDEX('AEO 46'!71:71,0,MATCH(About!$B$83,'AEO 46'!1:1,0)))*1000</f>
-        <v/>
-      </c>
-      <c r="D2" s="20">
-        <f>SUM(INDEX('AEO 46'!68:68,MATCH(About!$B$83,'AEO 46'!1:1,0)),INDEX('AEO 46'!72:72,MATCH(About!$B$83,'AEO 46'!1:1,0)))*1000</f>
-        <v/>
-      </c>
-      <c r="E2" s="20">
-        <f>INDEX('AEO 46'!69:69,MATCH(About!$B$83,'AEO 46'!$1:$1,0))*1000</f>
-        <v/>
-      </c>
-      <c r="F2" s="20">
-        <f>INDEX('AEO 46'!74:74,MATCH(About!$B$83,'AEO 46'!$1:$1,0))*10^6+INDEX('AEO 46'!75:75,MATCH(About!$B$83,'AEO 46'!$1:$1,0))*10^6</f>
-        <v/>
-      </c>
-      <c r="G2" s="20">
-        <f>SUM(INDEX('AEO 46'!70:70,0,MATCH(About!$B$83,'AEO 46'!1:1,0)))*1000</f>
-        <v/>
-      </c>
-      <c r="H2">
-        <f>SUM(INDEX('AEO 46'!76:76,0,MATCH(About!$B$83,'AEO 46'!1:1,0)))*1000</f>
-        <v/>
+      <c r="B2" s="20" t="n">
+        <v>6811</v>
+      </c>
+      <c r="C2" s="20" t="n">
+        <v>8385</v>
+      </c>
+      <c r="D2" s="20" t="n">
+        <v>3269118</v>
+      </c>
+      <c r="E2" s="20" t="n">
+        <v>53483</v>
+      </c>
+      <c r="F2" s="20" t="n">
+        <v>8344</v>
+      </c>
+      <c r="G2" s="20" t="n">
+        <v>17549</v>
+      </c>
+      <c r="H2" t="n">
+        <v>273</v>
       </c>
       <c r="I2" s="115" t="n"/>
       <c r="J2" s="20" t="n"/>
@@ -3094,33 +3076,26 @@
           <t>HDVs</t>
         </is>
       </c>
-      <c r="B3">
-        <f>SUM(INDEX('AEO 50'!$142:$142,MATCH(About!$B$83,'AEO 50'!$1:$1,0)),INDEX('AEO 50'!$153:$153,MATCH(About!$B$83,'AEO 50'!$1:$1,0)),INDEX('AEO 50'!$164:$164,MATCH(About!$B$83,'AEO 50'!$1:$1,0)))*10^6</f>
-        <v/>
-      </c>
-      <c r="C3">
-        <f>SUM(INDEX('AEO 50'!$140:$140,MATCH(About!$B$83,'AEO 50'!$1:$1,0)),INDEX('AEO 50'!$151:$151,MATCH(About!$B$83,'AEO 50'!$1:$1,0)),INDEX('AEO 50'!$162:$162,MATCH(About!$B$83,'AEO 50'!$1:$1,0)))*10^6</f>
-        <v/>
-      </c>
-      <c r="D3">
-        <f>SUM(INDEX('AEO 50'!$138:$138,MATCH(About!$B$83,'AEO 50'!$1:$1,0)),INDEX('AEO 50'!$141:$141,MATCH(About!$B$83,'AEO 50'!$1:$1,0)),INDEX('AEO 50'!$149:$149,MATCH(About!$B$83,'AEO 50'!$1:$1,0)),INDEX('AEO 50'!$152:$152,MATCH(About!$B$83,'AEO 50'!$1:$1,0)),INDEX('AEO 50'!$160:$160,MATCH(About!$B$83,'AEO 50'!$1:$1,0)),INDEX('AEO 50'!$163:$163,MATCH(About!$B$83,'AEO 50'!$1:$1,0)))*10^6</f>
-        <v/>
-      </c>
-      <c r="E3">
-        <f>SUM(INDEX('AEO 50'!$137:$137,MATCH(About!$B$83,'AEO 50'!$1:$1,0)),INDEX('AEO 50'!$148:$148,MATCH(About!$B$83,'AEO 50'!$1:$1,0)),INDEX('AEO 50'!$159:$159,MATCH(About!$B$83,'AEO 50'!$1:$1,0)))*10^6</f>
-        <v/>
-      </c>
-      <c r="F3">
-        <f>SUM(SUM(INDEX('AEO 50'!$143:$144,0,MATCH(About!$B$83,'AEO 50'!1:1,0))),SUM(INDEX('AEO 50'!$154:$155,0,MATCH(About!$B$83,'AEO 50'!1:1,0))),SUM(INDEX('AEO 50'!$165:$166,0,MATCH(About!$B$83,'AEO 50'!1:1,0))))*10^6</f>
-        <v/>
-      </c>
-      <c r="G3" s="20">
-        <f>SUM(INDEX('AEO 50'!$139:$139,MATCH(About!$B$83,'AEO 50'!$1:$1,0)),INDEX('AEO 50'!$150:$150,MATCH(About!$B$83,'AEO 50'!$1:$1,0)),INDEX('AEO 50'!$161:$161,MATCH(About!$B$83,'AEO 50'!$1:$1,0)))*10^6</f>
-        <v/>
-      </c>
-      <c r="H3" s="20">
-        <f>SUM(INDEX('AEO 50'!$145:$145,MATCH(About!$B$83,'AEO 50'!$1:$1,0)),INDEX('AEO 50'!$156:$156,MATCH(About!$B$83,'AEO 50'!$1:$1,0)),INDEX('AEO 50'!$167:$167,MATCH(About!$B$83,'AEO 50'!$1:$1,0)))*10^6</f>
-        <v/>
+      <c r="B3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1131</v>
+      </c>
+      <c r="D3" t="n">
+        <v>50075</v>
+      </c>
+      <c r="E3" t="n">
+        <v>127237</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="20" t="n">
+        <v>2247</v>
+      </c>
+      <c r="H3" s="20" t="n">
+        <v>0</v>
       </c>
       <c r="J3" s="20" t="n"/>
     </row>
@@ -3139,9 +3114,8 @@
       <c r="D4" t="n">
         <v>0</v>
       </c>
-      <c r="E4" s="13">
-        <f>INDEX('AEO 49'!$184:$184,MATCH(About!$B$83,'AEO 49'!$1:$1,0))</f>
-        <v/>
+      <c r="E4" s="13" t="n">
+        <v>8</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -3160,7 +3134,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3894.36</v>
+        <v>3894</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -3169,7 +3143,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="20" t="n">
-        <v>3741.64</v>
+        <v>3742</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -3237,7 +3211,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -79414,9 +79387,8 @@
       <c r="AI4" s="49" t="n">
         <v>7141</v>
       </c>
-      <c r="AJ4" s="79">
-        <f>TREND(AE4:AI4,AE2:AI2,AJ2)</f>
-        <v/>
+      <c r="AJ4" s="79" t="n">
+        <v>7235.399999999994</v>
       </c>
     </row>
     <row r="5" ht="16.5" customFormat="1" customHeight="1" s="25">
@@ -80661,13 +80633,11 @@
       <c r="AH14" s="55" t="n">
         <v>976161</v>
       </c>
-      <c r="AI14" s="73">
-        <f>TREND(AD14:AH14,AD2:AH2,AI2)</f>
-        <v/>
-      </c>
-      <c r="AJ14" s="73">
-        <f>TREND(AE14:AI14,AE2:AI2,AJ2)</f>
-        <v/>
+      <c r="AI14" s="73" t="n">
+        <v>1007529.274306253</v>
+      </c>
+      <c r="AJ14" s="73" t="n">
+        <v>1038863.030252293</v>
       </c>
       <c r="AK14" s="49" t="n"/>
     </row>
@@ -80820,9 +80790,8 @@
       <c r="AI16" s="60" t="n">
         <v>63759</v>
       </c>
-      <c r="AJ16" s="25">
-        <f>TREND(AE16:AI16,$AE$2:$AI$2,$AJ$2)</f>
-        <v/>
+      <c r="AJ16" s="25" t="n">
+        <v>62382.69999999995</v>
       </c>
     </row>
     <row r="17" ht="16.5" customFormat="1" customHeight="1" s="25">
@@ -80933,9 +80902,8 @@
       <c r="AI17" s="60" t="n">
         <v>2557</v>
       </c>
-      <c r="AJ17" s="25">
-        <f>TREND(AE17:AI17,$AE$2:$AI$2,$AJ$2)</f>
-        <v/>
+      <c r="AJ17" s="25" t="n">
+        <v>2436.5</v>
       </c>
     </row>
     <row r="18" ht="16.5" customFormat="1" customHeight="1" s="25">
@@ -81046,9 +81014,8 @@
       <c r="AI18" s="60" t="n">
         <v>10705</v>
       </c>
-      <c r="AJ18" s="25">
-        <f>TREND(AE18:AI18,$AE$2:$AI$2,$AJ$2)</f>
-        <v/>
+      <c r="AJ18" s="25" t="n">
+        <v>10891.80000000002</v>
       </c>
     </row>
     <row r="19" ht="16.5" customFormat="1" customHeight="1" s="25">
@@ -81159,9 +81126,8 @@
       <c r="AI19" s="60" t="n">
         <v>539</v>
       </c>
-      <c r="AJ19" s="25">
-        <f>TREND(AE19:AI19,$AE$2:$AI$2,$AJ$2)</f>
-        <v/>
+      <c r="AJ19" s="25" t="n">
+        <v>576.2000000000003</v>
       </c>
     </row>
     <row r="20" ht="16.5" customFormat="1" customHeight="1" s="25">
@@ -81280,9 +81246,8 @@
       <c r="AI20" s="60" t="n">
         <v>7129</v>
       </c>
-      <c r="AJ20" s="25">
-        <f>TREND(AE20:AI20,$AE$2:$AI$2,$AJ$2)</f>
-        <v/>
+      <c r="AJ20" s="25" t="n">
+        <v>7150.7</v>
       </c>
     </row>
     <row r="21" ht="16.5" customFormat="1" customHeight="1" s="25">
@@ -81403,9 +81368,8 @@
       <c r="AI21" s="60" t="n">
         <v>33012</v>
       </c>
-      <c r="AJ21" s="25">
-        <f>TREND(AE21:AI21,$AE$2:$AI$2,$AJ$2)</f>
-        <v/>
+      <c r="AJ21" s="25" t="n">
+        <v>33811</v>
       </c>
     </row>
     <row r="22" ht="16.5" customFormat="1" customHeight="1" s="25">
@@ -81526,9 +81490,8 @@
       <c r="AI22" s="60" t="n">
         <v>18104</v>
       </c>
-      <c r="AJ22" s="25">
-        <f>TREND(AE22:AI22,$AE$2:$AI$2,$AJ$2)</f>
-        <v/>
+      <c r="AJ22" s="25" t="n">
+        <v>17807.8</v>
       </c>
     </row>
     <row r="23" ht="16.5" customFormat="1" customHeight="1" s="46">
@@ -81681,9 +81644,8 @@
       <c r="AI24" s="56" t="n">
         <v>306268</v>
       </c>
-      <c r="AJ24" s="25">
-        <f>TREND(AE24:AI24,$AE$2:$AI$2,$AJ$2)</f>
-        <v/>
+      <c r="AJ24" s="25" t="n">
+        <v>282127.700000003</v>
       </c>
     </row>
     <row r="25" ht="16.5" customFormat="1" customHeight="1" s="25">
@@ -81794,9 +81756,8 @@
       <c r="AI25" s="56" t="n">
         <v>26547</v>
       </c>
-      <c r="AJ25" s="25">
-        <f>TREND(AE25:AI25,$AE$2:$AI$2,$AJ$2)</f>
-        <v/>
+      <c r="AJ25" s="25" t="n">
+        <v>27305.59999999998</v>
       </c>
     </row>
     <row r="26" ht="16.5" customFormat="1" customHeight="1" s="25">
@@ -82147,9 +82108,8 @@
       <c r="AI28" s="56" t="n">
         <v>1405</v>
       </c>
-      <c r="AJ28" s="25">
-        <f>TREND(AE28:AI28,$AE$2:$AI$2,$AJ$2)</f>
-        <v/>
+      <c r="AJ28" s="25" t="n">
+        <v>1389.900000000001</v>
       </c>
     </row>
     <row r="29" ht="16.5" customFormat="1" customHeight="1" s="25">
@@ -82266,9 +82226,8 @@
       <c r="AI29" s="56" t="n">
         <v>419</v>
       </c>
-      <c r="AJ29" s="25">
-        <f>TREND(AE29:AI29,$AE$2:$AI$2,$AJ$2)</f>
-        <v/>
+      <c r="AJ29" s="25" t="n">
+        <v>426.8000000000002</v>
       </c>
     </row>
     <row r="30" ht="16.5" customFormat="1" customHeight="1" s="46">
@@ -82423,9 +82382,8 @@
       <c r="AI31" s="56" t="n">
         <v>33128</v>
       </c>
-      <c r="AJ31" s="25">
-        <f>TREND(AE31:AI31,$AE$2:$AI$2,$AJ$2)</f>
-        <v/>
+      <c r="AJ31" s="25" t="n">
+        <v>33921.29999999981</v>
       </c>
     </row>
     <row r="32" ht="16.5" customFormat="1" customHeight="1" s="25">
@@ -82538,9 +82496,8 @@
       <c r="AI32" s="56" t="n">
         <v>9411</v>
       </c>
-      <c r="AJ32" s="25">
-        <f>TREND(AE32:AI32,$AE$2:$AI$2,$AJ$2)</f>
-        <v/>
+      <c r="AJ32" s="25" t="n">
+        <v>9597.299999999988</v>
       </c>
     </row>
     <row r="33" ht="32.25" customFormat="1" customHeight="1" s="25">
@@ -82651,9 +82608,8 @@
       <c r="AI33" s="49" t="n">
         <v>176</v>
       </c>
-      <c r="AJ33" s="25">
-        <f>TREND(AE33:AI33,$AE$2:$AI$2,$AJ$2)</f>
-        <v/>
+      <c r="AJ33" s="25" t="n">
+        <v>166.5999999999995</v>
       </c>
     </row>
     <row r="34" ht="16.5" customFormat="1" customHeight="1" s="25" thickBot="1">
@@ -82764,9 +82720,8 @@
       <c r="AI34" s="66" t="n">
         <v>11961568</v>
       </c>
-      <c r="AJ34" s="25">
-        <f>TREND(AE34:AI34,$AE$2:$AI$2,$AJ$2)</f>
-        <v/>
+      <c r="AJ34" s="25" t="n">
+        <v>11887771.1</v>
       </c>
     </row>
     <row r="35" ht="12.75" customFormat="1" customHeight="1" s="70">

</xml_diff>